<commit_message>
Adds -c flag, updates anno-splice events to CPU pool
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t xml:space="preserve">Iteration</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Modifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample</t>
   </si>
   <si>
     <r>
@@ -61,6 +64,9 @@
     <t xml:space="preserve">Modified samtools directory for my system</t>
   </si>
   <si>
+    <t xml:space="preserve">Sample Input from GitHub</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -109,10 +115,64 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">0.11 min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Added CPU pooling to MakeFullDictionary</t>
+    <t xml:space="preserve">0.09min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added CPU pooling to MakeDict and splicing events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPU Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.40min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.28min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GitHub Test Samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.26min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.81min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BT549 from Coombs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New (v2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.35min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.21min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.14min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.11min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.07min</t>
   </si>
 </sst>
 </file>
@@ -123,7 +183,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -158,6 +218,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -220,7 +285,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,6 +306,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -249,7 +318,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -330,16 +407,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="43.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="43.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -355,90 +443,316 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="6" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="C4" s="9" t="n">
         <v>0.725</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="D5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="9" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="10" t="n">
+        <v>0.475</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="10" t="n">
+        <v>0.475</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="9" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="10" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="10" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="D13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="D14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
+      <c r="D15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="D16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="D17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="D18" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>